<commit_message>
Added new file final figure and logistic regression
</commit_message>
<xml_diff>
--- a/Input/Demographic.xlsx
+++ b/Input/Demographic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD-Tomer\Projects\Rapamycin\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76417C6D-0DE0-4B47-B696-A01B2C55DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63C1AE-E533-4932-9A7B-12190AE9E7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{5217D417-85FB-476E-B620-EB60C421C6C5}"/>
   </bookViews>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>survival_group</t>
   </si>
   <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>group</t>
   </si>
   <si>
     <t>Group</t>
@@ -417,7 +414,7 @@
   <dimension ref="A1:B135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,12 +452,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>

</xml_diff>